<commit_message>
Import Job Layout Show Job Available to Import and Duplicated Job
</commit_message>
<xml_diff>
--- a/LaborCostAnalysis/wwwroot/files/Jobs.xlsx
+++ b/LaborCostAnalysis/wwwroot/files/Jobs.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550F7960-8EAA-40AF-8CCE-78DB02556ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15780" windowHeight="6660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="240">
   <si>
     <t>Job_Name</t>
   </si>
@@ -717,12 +716,30 @@
   </si>
   <si>
     <t>E-6203 install IE&amp;EE work  Project (TMMA)</t>
+  </si>
+  <si>
+    <t>J99-9999</t>
+  </si>
+  <si>
+    <t>TEST EXCEL</t>
+  </si>
+  <si>
+    <t>J99-9998</t>
+  </si>
+  <si>
+    <t>TEST EXCEL 2</t>
+  </si>
+  <si>
+    <t>J99-9997</t>
+  </si>
+  <si>
+    <t>TEST EXCEL 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -832,7 +849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -866,6 +883,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,23 +979,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1011,23 +1014,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1203,11 +1189,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G118"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2538,6 +2524,39 @@
         <v>2021</v>
       </c>
     </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B119" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C119" s="3">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B120" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="C120" s="3">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B121" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C121" s="3">
+        <v>2021</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Check Duplicate Import Job, Labor Cost
</commit_message>
<xml_diff>
--- a/LaborCostAnalysis/wwwroot/files/Jobs.xlsx
+++ b/LaborCostAnalysis/wwwroot/files/Jobs.xlsx
@@ -4,17 +4,28 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15780" windowHeight="6660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="234">
   <si>
     <t>Job_Name</t>
   </si>
@@ -220,18 +231,12 @@
     <t>อำนาจเจริญ</t>
   </si>
   <si>
-    <t>UAW (1) 16-31JAN 2020 (สังคม)</t>
-  </si>
-  <si>
     <t>J19-0853</t>
   </si>
   <si>
     <t>นตและอ้อย 1-31 JAN 2020 (นศ.)</t>
   </si>
   <si>
-    <t>Covestro 1-29 FEB 2020 (นศ.)</t>
-  </si>
-  <si>
     <t>J19-1491</t>
   </si>
   <si>
@@ -718,22 +723,10 @@
     <t>E-6203 install IE&amp;EE work  Project (TMMA)</t>
   </si>
   <si>
-    <t>J99-9999</t>
-  </si>
-  <si>
-    <t>TEST EXCEL</t>
-  </si>
-  <si>
-    <t>J99-9998</t>
-  </si>
-  <si>
-    <t>TEST EXCEL 2</t>
-  </si>
-  <si>
-    <t>J99-9997</t>
-  </si>
-  <si>
-    <t>TEST EXCEL 3</t>
+    <t>Duplicate 1</t>
+  </si>
+  <si>
+    <t>Duplicate 2</t>
   </si>
 </sst>
 </file>
@@ -849,7 +842,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -883,9 +876,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,10 +1180,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G121"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,10 +1581,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C34" s="1">
         <v>2021</v>
@@ -1602,10 +1592,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C35" s="1">
         <v>2021</v>
@@ -1613,10 +1603,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C36" s="1">
         <v>2021</v>
@@ -1624,10 +1614,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C37" s="1">
         <v>2021</v>
@@ -1635,10 +1625,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C38" s="1">
         <v>2021</v>
@@ -1646,10 +1636,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C39" s="1">
         <v>2021</v>
@@ -1657,10 +1647,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C40" s="1">
         <v>2021</v>
@@ -1668,10 +1658,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C41" s="1">
         <v>2021</v>
@@ -1679,10 +1669,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C42" s="1">
         <v>2021</v>
@@ -1690,10 +1680,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C43" s="1">
         <v>2021</v>
@@ -1701,10 +1691,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C44" s="1">
         <v>2021</v>
@@ -1712,10 +1702,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C45" s="1">
         <v>2021</v>
@@ -1723,10 +1713,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C46" s="1">
         <v>2021</v>
@@ -1734,10 +1724,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C47" s="1">
         <v>2021</v>
@@ -1745,10 +1735,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C48" s="1">
         <v>2021</v>
@@ -1756,10 +1746,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C49" s="1">
         <v>2021</v>
@@ -1767,10 +1757,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C50" s="1">
         <v>2021</v>
@@ -1778,10 +1768,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C51" s="1">
         <v>2021</v>
@@ -1789,10 +1779,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C52" s="1">
         <v>2021</v>
@@ -1800,10 +1790,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C53" s="1">
         <v>2021</v>
@@ -1811,10 +1801,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C54" s="1">
         <v>2021</v>
@@ -1822,10 +1812,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C55" s="1">
         <v>2021</v>
@@ -1833,10 +1823,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C56" s="1">
         <v>2021</v>
@@ -1844,10 +1834,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C57" s="1">
         <v>2021</v>
@@ -1855,10 +1845,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C58" s="1">
         <v>2021</v>
@@ -1866,10 +1856,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C59" s="1">
         <v>2021</v>
@@ -1877,10 +1867,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C60" s="1">
         <v>2021</v>
@@ -1888,10 +1878,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C61" s="1">
         <v>2021</v>
@@ -1899,10 +1889,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C62" s="1">
         <v>2021</v>
@@ -1910,10 +1900,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C63" s="1">
         <v>2021</v>
@@ -1921,10 +1911,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C64" s="1">
         <v>2021</v>
@@ -1932,10 +1922,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C65" s="1">
         <v>2021</v>
@@ -1943,10 +1933,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C66" s="1">
         <v>2021</v>
@@ -1954,10 +1944,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C67" s="1">
         <v>2021</v>
@@ -1965,10 +1955,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C68" s="1">
         <v>2021</v>
@@ -1976,10 +1966,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C69" s="1">
         <v>2021</v>
@@ -1987,10 +1977,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C70" s="1">
         <v>2021</v>
@@ -1998,10 +1988,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C71" s="1">
         <v>2021</v>
@@ -2009,10 +1999,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C72" s="1">
         <v>2021</v>
@@ -2020,10 +2010,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C73" s="1">
         <v>2021</v>
@@ -2031,10 +2021,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C74" s="1">
         <v>2021</v>
@@ -2042,10 +2032,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C75" s="1">
         <v>2021</v>
@@ -2053,10 +2043,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C76" s="1">
         <v>2021</v>
@@ -2064,10 +2054,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C77" s="1">
         <v>2021</v>
@@ -2075,10 +2065,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C78" s="1">
         <v>2021</v>
@@ -2086,10 +2076,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C79" s="1">
         <v>2021</v>
@@ -2097,10 +2087,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C80" s="1">
         <v>2021</v>
@@ -2108,10 +2098,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C81" s="1">
         <v>2021</v>
@@ -2119,10 +2109,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C82" s="1">
         <v>2021</v>
@@ -2130,10 +2120,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C83" s="1">
         <v>2021</v>
@@ -2141,21 +2131,21 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C84" s="1">
         <v>2021</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>169</v>
+      <c r="A85" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>171</v>
       </c>
       <c r="C85" s="1">
         <v>2021</v>
@@ -2163,21 +2153,21 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C86" s="1">
         <v>2021</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B87" s="12" t="s">
-        <v>173</v>
+      <c r="A87" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>175</v>
       </c>
       <c r="C87" s="1">
         <v>2021</v>
@@ -2185,10 +2175,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C88" s="1">
         <v>2021</v>
@@ -2196,10 +2186,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C89" s="1">
         <v>2021</v>
@@ -2207,10 +2197,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C90" s="1">
         <v>2021</v>
@@ -2218,10 +2208,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C91" s="1">
         <v>2021</v>
@@ -2229,10 +2219,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="C92" s="1">
         <v>2021</v>
@@ -2240,10 +2230,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C93" s="1">
         <v>2021</v>
@@ -2251,10 +2241,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C94" s="1">
         <v>2021</v>
@@ -2262,10 +2252,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C95" s="1">
         <v>2021</v>
@@ -2273,10 +2263,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C96" s="1">
         <v>2021</v>
@@ -2284,10 +2274,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C97" s="1">
         <v>2021</v>
@@ -2295,10 +2285,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C98" s="1">
         <v>2021</v>
@@ -2306,10 +2296,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="C99" s="1">
         <v>2021</v>
@@ -2317,10 +2307,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C100" s="1">
         <v>2021</v>
@@ -2328,10 +2318,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="C101" s="1">
         <v>2021</v>
@@ -2339,10 +2329,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C102" s="1">
         <v>2021</v>
@@ -2350,10 +2340,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C103" s="1">
         <v>2021</v>
@@ -2361,10 +2351,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C104" s="1">
         <v>2021</v>
@@ -2372,10 +2362,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C105" s="1">
         <v>2021</v>
@@ -2383,10 +2373,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C106" s="1">
         <v>2021</v>
@@ -2394,10 +2384,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C107" s="1">
         <v>2021</v>
@@ -2405,10 +2395,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C108" s="1">
         <v>2021</v>
@@ -2416,10 +2406,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C109" s="1">
         <v>2021</v>
@@ -2427,10 +2417,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C110" s="1">
         <v>2021</v>
@@ -2438,10 +2428,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C111" s="1">
         <v>2021</v>
@@ -2449,21 +2439,21 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C112" s="1">
         <v>2021</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>223</v>
+      <c r="A113" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>225</v>
       </c>
       <c r="C113" s="1">
         <v>2021</v>
@@ -2471,21 +2461,21 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C114" s="1">
         <v>2021</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="B115" s="14" t="s">
-        <v>227</v>
+      <c r="A115" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>229</v>
       </c>
       <c r="C115" s="1">
         <v>2021</v>
@@ -2493,10 +2483,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C116" s="1">
         <v>2021</v>
@@ -2507,7 +2497,7 @@
         <v>230</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C117" s="1">
         <v>2021</v>
@@ -2515,45 +2505,12 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>233</v>
       </c>
       <c r="C118" s="1">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="B119" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="C119" s="3">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B120" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="C120" s="3">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B121" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="C121" s="3">
         <v>2021</v>
       </c>
     </row>

</xml_diff>